<commit_message>
push the update code
</commit_message>
<xml_diff>
--- a/com.healthCare.arogya/testData.xlsx
+++ b/com.healthCare.arogya/testData.xlsx
@@ -1,25 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15300" windowHeight="6540" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17220" windowHeight="7716" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="1" r:id="rId1"/>
-    <sheet name="ArogyaBooking" sheetId="2" r:id="rId2"/>
-    <sheet name="Paymentdetails" sheetId="3" r:id="rId3"/>
-    <sheet name="PaymentPage" sheetId="4" r:id="rId4"/>
-    <sheet name="Login" sheetId="5" r:id="rId5"/>
+    <sheet name="DoctorLogin" sheetId="7" r:id="rId2"/>
+    <sheet name="ArogyaBooking" sheetId="2" r:id="rId3"/>
+    <sheet name="Paymentdetails" sheetId="3" r:id="rId4"/>
+    <sheet name="PaymentPage" sheetId="4" r:id="rId5"/>
+    <sheet name="Login" sheetId="5" r:id="rId6"/>
+    <sheet name="AppoinmantDetails" sheetId="6" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="124519"/>
-  <oleSize ref="A1:N20"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:Q25"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="54">
   <si>
     <t>TC_ID</t>
   </si>
@@ -136,13 +138,58 @@
   </si>
   <si>
     <t>Anshikadubey@gmail.com</t>
+  </si>
+  <si>
+    <t>TC_01</t>
+  </si>
+  <si>
+    <t>medication</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cinnamon </t>
+  </si>
+  <si>
+    <t>Cinnamon powder can be added to food or consumed with warm water</t>
+  </si>
+  <si>
+    <t>Fenugreek</t>
+  </si>
+  <si>
+    <t>Soak a teaspoon of fenugreek seeds overnight and consume them in the morning</t>
+  </si>
+  <si>
+    <t>userName</t>
+  </si>
+  <si>
+    <t>specialization</t>
+  </si>
+  <si>
+    <t>anshikadubey144@gmail.com</t>
+  </si>
+  <si>
+    <t>Kaya Chikitsa</t>
+  </si>
+  <si>
+    <t>Anshika@7276</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>slmcrNo</t>
+  </si>
+  <si>
+    <t>docPassword</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,8 +204,21 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -180,6 +240,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -215,7 +287,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -227,6 +299,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -234,6 +316,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -280,7 +370,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -312,9 +402,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -346,6 +437,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -521,23 +613,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" customWidth="1"/>
+    <col min="3" max="3" width="24.44140625" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -554,7 +646,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -571,7 +663,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -603,20 +695,104 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10.44140625" customWidth="1"/>
+    <col min="3" max="3" width="25.77734375" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="16.21875" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" customWidth="1"/>
+    <col min="7" max="7" width="16.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="F2" r:id="rId2"/>
+    <hyperlink ref="G2" r:id="rId3" display="Anshika@7275"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" customWidth="1"/>
+    <col min="3" max="3" width="21.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
@@ -627,7 +803,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -638,7 +814,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -654,21 +830,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
@@ -682,7 +858,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -696,7 +872,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -708,58 +884,6 @@
       </c>
       <c r="D3" s="6" t="s">
         <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -768,20 +892,72 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="28.5703125" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="28.5546875" customWidth="1"/>
+    <col min="3" max="3" width="20.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -792,7 +968,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -803,7 +979,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -823,4 +999,66 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="11.77734375" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>123456</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>789012</v>
+      </c>
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>